<commit_message>
add delegation interfaces design
</commit_message>
<xml_diff>
--- a/Application.xlsx
+++ b/Application.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutosarTutorial\ArxmlTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952712A6-72B6-4C89-866B-A747D645D980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2443C230-FB5D-4FF9-BF7D-E510C7C3141F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EBD56D4D-7AAB-47EC-B02E-89E578045FA0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{EBD56D4D-7AAB-47EC-B02E-89E578045FA0}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTypes" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="84">
   <si>
     <t>TypeName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -232,10 +232,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TASK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TASK_10MS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -252,10 +248,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PORT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>P_VehicleConditions</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -301,6 +293,74 @@
   </si>
   <si>
     <t>SWC2, Delegation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Task</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Port</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ComponentType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>APP-SWC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DELEGATION</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SW_Composition1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>APP-COMP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SWC2, SW_Composition1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P_SA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P_SB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P_SC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GeneralInterface</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DefaultPortAccess</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Receive Port</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P_SomeBody</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -360,7 +420,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -562,10 +622,10 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -575,27 +635,114 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
@@ -604,22 +751,7 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -628,7 +760,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -719,22 +851,46 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1053,8 +1209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A675E1F-9C03-4EE3-AE97-C268A8F23FBE}">
   <dimension ref="B1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1356,10 +1512,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA44D0C-18C8-469C-9219-A37B0C48C99E}">
-  <dimension ref="B2:D13"/>
+  <dimension ref="B2:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1464,6 +1620,22 @@
       <c r="C13" s="8"/>
       <c r="D13" s="26"/>
     </row>
+    <row r="14" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B14" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="42" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="7"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="26"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1472,216 +1644,363 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A1755F-5E81-4222-BC5B-9CFC616875A8}">
-  <dimension ref="B1:G18"/>
+  <dimension ref="B1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="11.75" customWidth="1"/>
-    <col min="4" max="4" width="27.75" customWidth="1"/>
-    <col min="5" max="5" width="15.25" customWidth="1"/>
-    <col min="6" max="6" width="21.5" customWidth="1"/>
-    <col min="7" max="7" width="21.375" customWidth="1"/>
+    <col min="2" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="11.75" customWidth="1"/>
+    <col min="5" max="6" width="27.75" customWidth="1"/>
+    <col min="7" max="7" width="20.5" customWidth="1"/>
+    <col min="8" max="8" width="15.25" customWidth="1"/>
+    <col min="9" max="9" width="21.5" customWidth="1"/>
+    <col min="10" max="10" width="40.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="30" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B3" s="33"/>
-    </row>
-    <row r="4" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B4" s="32" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="34"/>
-    </row>
-    <row r="6" spans="2:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B3" s="32"/>
+    </row>
+    <row r="4" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B4" s="31" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="39"/>
+    </row>
+    <row r="6" spans="2:10" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="40" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="E6" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="28" t="s">
-        <v>55</v>
-      </c>
       <c r="F6" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="29" t="s">
+      <c r="J6" s="29" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
-      <c r="C7" s="2"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="2:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B8" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" s="16"/>
+      <c r="J8" s="17"/>
+    </row>
+    <row r="9" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B9" s="15"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" s="16" t="s">
+      <c r="F9" s="16"/>
+      <c r="G9" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="H9" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="16"/>
-      <c r="G8" s="17"/>
-    </row>
-    <row r="9" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B9" s="15"/>
-      <c r="C9" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="16"/>
-      <c r="G9" s="17"/>
-    </row>
-    <row r="10" spans="2:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="I9" s="16"/>
+      <c r="J9" s="17"/>
+    </row>
+    <row r="10" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B10" s="15"/>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="35"/>
+      <c r="D10" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B11" s="15"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B12" s="15"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B11" s="15"/>
-      <c r="C11" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16" t="s">
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B12" s="15"/>
-      <c r="C12" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="J12" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" s="4"/>
-      <c r="C13" s="5"/>
+      <c r="C13" s="36"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
-      <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="2:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B14" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="16"/>
+      <c r="J14" s="17"/>
+    </row>
+    <row r="15" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B15" s="15"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="H15" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="16"/>
-      <c r="G14" s="17"/>
-    </row>
-    <row r="15" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B15" s="15"/>
-      <c r="C15" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F15" s="16"/>
-      <c r="G15" s="17"/>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="I15" s="16"/>
+      <c r="J15" s="17"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" s="4"/>
-      <c r="C16" s="5"/>
+      <c r="C16" s="36"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="6"/>
-    </row>
-    <row r="17" spans="2:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="B17" s="35" t="s">
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="6"/>
+    </row>
+    <row r="17" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B17" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="J17" s="17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B18" s="15"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" s="16"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="J18" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B19" s="15"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="J19" s="17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B20" s="4"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="6"/>
+    </row>
+    <row r="21" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B21" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16" t="s">
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="G17" s="17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="9"/>
+      <c r="J21" s="17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B22" s="33"/>
+      <c r="C22" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41" t="s">
+        <v>83</v>
+      </c>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="J22" s="42"/>
+    </row>
+    <row r="23" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="7"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add python scripts for datatype import
</commit_message>
<xml_diff>
--- a/Application.xlsx
+++ b/Application.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutosarTutorial\ArxmlTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2443C230-FB5D-4FF9-BF7D-E510C7C3141F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15773D3A-61BA-4031-9F56-2DCD0CAD52C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{EBD56D4D-7AAB-47EC-B02E-89E578045FA0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EBD56D4D-7AAB-47EC-B02E-89E578045FA0}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTypes" sheetId="1" r:id="rId1"/>
     <sheet name="Interfaces" sheetId="2" r:id="rId2"/>
-    <sheet name="SWC" sheetId="3" r:id="rId3"/>
+    <sheet name="SWC_Composition" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -1209,8 +1209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A675E1F-9C03-4EE3-AE97-C268A8F23FBE}">
   <dimension ref="B1:E32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1646,8 +1646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A1755F-5E81-4222-BC5B-9CFC616875A8}">
   <dimension ref="B1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
data types arxml generated
</commit_message>
<xml_diff>
--- a/Application.xlsx
+++ b/Application.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutosarTutorial\ArxmlTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15773D3A-61BA-4031-9F56-2DCD0CAD52C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6EC35A-A42F-47CE-8667-D8AABD68C655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EBD56D4D-7AAB-47EC-B02E-89E578045FA0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EBD56D4D-7AAB-47EC-B02E-89E578045FA0}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTypes" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="87">
   <si>
     <t>TypeName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -361,6 +361,18 @@
   </si>
   <si>
     <t>P_SomeBody</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Uint32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unsigned long</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bit Size</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -760,7 +772,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -892,6 +904,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1207,10 +1222,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A675E1F-9C03-4EE3-AE97-C268A8F23FBE}">
-  <dimension ref="B1:E32"/>
+  <dimension ref="B1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1218,7 +1233,7 @@
     <col min="1" max="1" width="6.125" customWidth="1"/>
     <col min="2" max="2" width="16.875" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="21.875" customWidth="1"/>
     <col min="5" max="5" width="19.25" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
     <col min="8" max="9" width="9" customWidth="1"/>
@@ -1232,14 +1247,18 @@
       <c r="C2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="29" t="s">
+      <c r="D2" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="29" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B3" s="12"/>
       <c r="C3" s="13"/>
-      <c r="D3" s="14"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="14"/>
     </row>
     <row r="4" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B4" s="15" t="s">
@@ -1248,200 +1267,224 @@
       <c r="C4" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="44">
+        <v>8</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="20"/>
+      <c r="B5" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="44">
+        <v>8</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B6" s="15" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="44">
+        <v>16</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B7" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="44">
+        <v>32</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="23"/>
+    </row>
+    <row r="9" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="1"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B12" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B13" s="15"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="17">
         <v>3</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B7" s="18"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="20"/>
-    </row>
-    <row r="8" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B8" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="21"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="23"/>
-    </row>
-    <row r="10" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="29" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="1"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B13" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="17">
-        <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B14" s="15"/>
       <c r="C14" s="16"/>
       <c r="D14" s="24" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E14" s="17">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B15" s="15"/>
       <c r="C15" s="16"/>
       <c r="D15" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E15" s="17">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B16" s="15"/>
       <c r="C16" s="16"/>
       <c r="D16" s="24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E16" s="17">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B17" s="15"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="17">
-        <v>12</v>
-      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="20"/>
     </row>
     <row r="18" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B18" s="18"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="20"/>
+      <c r="B18" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="17">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B19" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>11</v>
-      </c>
+      <c r="B19" s="15"/>
+      <c r="C19" s="16"/>
       <c r="D19" s="24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E19" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B20" s="15"/>
       <c r="C20" s="16"/>
       <c r="D20" s="24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E20" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="7"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="9"/>
+    </row>
+    <row r="22" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="11"/>
+    </row>
+    <row r="23" spans="2:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" s="28" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B21" s="15"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="E21" s="17">
+      <c r="D23" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="1"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="2:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="B25" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="17" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="9"/>
-    </row>
-    <row r="23" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="D23" s="11"/>
-    </row>
-    <row r="24" spans="2:5" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" s="29" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B25" s="1"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="3"/>
-    </row>
     <row r="26" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B26" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="16" t="s">
-        <v>25</v>
-      </c>
+      <c r="B26" s="15"/>
+      <c r="C26" s="16"/>
       <c r="D26" s="16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E26" s="17" t="s">
         <v>2</v>
@@ -1451,57 +1494,47 @@
       <c r="B27" s="15"/>
       <c r="C27" s="16"/>
       <c r="D27" s="16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E27" s="17" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B28" s="15"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>2</v>
-      </c>
+      <c r="B28" s="18"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="20"/>
     </row>
     <row r="29" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B29" s="18"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="20"/>
+      <c r="B29" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="17" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="30" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B30" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" s="16" t="s">
-        <v>25</v>
-      </c>
+      <c r="B30" s="15"/>
+      <c r="C30" s="16"/>
       <c r="D30" s="16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="B31" s="15"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E31" s="17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="7"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="9"/>
+    <row r="31" spans="2:5" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="7"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add sw component system collection method
</commit_message>
<xml_diff>
--- a/Application.xlsx
+++ b/Application.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutosarTutorial\ArxmlTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F253B071-DD77-426E-9CE1-7D7661268F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905C6847-0B2A-42F5-A91C-CB2641F08B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{EBD56D4D-7AAB-47EC-B02E-89E578045FA0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{EBD56D4D-7AAB-47EC-B02E-89E578045FA0}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTypes" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="89">
   <si>
     <t>TypeName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1558,7 +1558,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FA44D0C-18C8-469C-9219-A37B0C48C99E}">
   <dimension ref="B2:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -1714,8 +1714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A1755F-5E81-4222-BC5B-9CFC616875A8}">
   <dimension ref="B1:J23"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2042,9 +2042,7 @@
     </row>
     <row r="22" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B22" s="33"/>
-      <c r="C22" s="37" t="s">
-        <v>71</v>
-      </c>
+      <c r="C22" s="37"/>
       <c r="D22" s="41" t="s">
         <v>68</v>
       </c>

</xml_diff>

<commit_message>
add component class and complete port creation
</commit_message>
<xml_diff>
--- a/Application.xlsx
+++ b/Application.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutosarTutorial\ArxmlTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A10F46-F6DF-4667-B4D8-1A5FD58FB347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42FEE28B-4174-439C-8E77-C2CEABB8951D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{EBD56D4D-7AAB-47EC-B02E-89E578045FA0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{EBD56D4D-7AAB-47EC-B02E-89E578045FA0}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTypes" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="90">
   <si>
     <t>TypeName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -212,10 +212,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Provide Port</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Receiver SWC</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -341,10 +337,6 @@
   </si>
   <si>
     <t>Yes</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Receive Port</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -378,6 +370,22 @@
   </si>
   <si>
     <t>ToplevelComposition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Direction</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Provider</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Receiver</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PortName</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1195,7 +1203,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E2" s="29" t="s">
         <v>5</v>
@@ -1251,7 +1259,7 @@
     </row>
     <row r="7" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B7" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>4</v>
@@ -1260,7 +1268,7 @@
         <v>32</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -1521,7 +1529,7 @@
         <v>15</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
@@ -1535,7 +1543,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>40</v>
@@ -1575,7 +1583,7 @@
         <v>34</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>36</v>
@@ -1605,7 +1613,7 @@
         <v>35</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D12" s="16" t="s">
         <v>38</v>
@@ -1622,13 +1630,13 @@
     </row>
     <row r="14" spans="2:5" ht="15" x14ac:dyDescent="0.2">
       <c r="B14" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="37" t="s">
         <v>75</v>
-      </c>
-      <c r="C14" s="34" t="s">
-        <v>84</v>
-      </c>
-      <c r="D14" s="37" t="s">
-        <v>76</v>
       </c>
       <c r="E14" s="38" t="s">
         <v>2</v>
@@ -1651,7 +1659,7 @@
   <dimension ref="B1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1659,8 +1667,9 @@
     <col min="2" max="2" width="20.625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="11.75" customWidth="1"/>
-    <col min="5" max="6" width="27.75" customWidth="1"/>
-    <col min="7" max="7" width="20.5" customWidth="1"/>
+    <col min="5" max="5" width="22.5" customWidth="1"/>
+    <col min="6" max="6" width="11.875" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
     <col min="8" max="8" width="15.25" customWidth="1"/>
     <col min="9" max="9" width="21.5" customWidth="1"/>
     <col min="10" max="10" width="40.625" customWidth="1"/>
@@ -1672,28 +1681,28 @@
         <v>44</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D2" s="28" t="s">
         <v>45</v>
       </c>
       <c r="E2" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="29" t="s">
         <v>46</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="H2" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="J2" s="29" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
@@ -1709,21 +1718,21 @@
     </row>
     <row r="4" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B4" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="16" t="s">
         <v>49</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>50</v>
       </c>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
       <c r="H4" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I4" s="16"/>
       <c r="J4" s="17"/>
@@ -1732,17 +1741,17 @@
       <c r="B5" s="15"/>
       <c r="C5" s="32"/>
       <c r="D5" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I5" s="16"/>
       <c r="J5" s="17"/>
@@ -1751,57 +1760,63 @@
       <c r="B6" s="15"/>
       <c r="C6" s="32"/>
       <c r="D6" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="16"/>
+        <v>54</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>87</v>
+      </c>
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
       <c r="I6" s="16" t="s">
         <v>39</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B7" s="15"/>
       <c r="C7" s="32"/>
       <c r="D7" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" s="16"/>
+        <v>55</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>87</v>
+      </c>
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
       <c r="I7" s="16" t="s">
         <v>34</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B8" s="15"/>
       <c r="C8" s="32"/>
       <c r="D8" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="F8" s="16"/>
+        <v>56</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>87</v>
+      </c>
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
       <c r="I8" s="16" t="s">
         <v>34</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
@@ -1817,21 +1832,21 @@
     </row>
     <row r="10" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B10" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
       <c r="H10" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I10" s="16"/>
       <c r="J10" s="17"/>
@@ -1840,17 +1855,17 @@
       <c r="B11" s="15"/>
       <c r="C11" s="32"/>
       <c r="D11" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I11" s="16"/>
       <c r="J11" s="17"/>
@@ -1868,63 +1883,69 @@
     </row>
     <row r="13" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B13" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="32" t="s">
-        <v>70</v>
-      </c>
       <c r="D13" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="F13" s="16"/>
+        <v>71</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>87</v>
+      </c>
       <c r="G13" s="16"/>
       <c r="H13" s="16"/>
       <c r="I13" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B14" s="15"/>
       <c r="C14" s="32"/>
       <c r="D14" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="F14" s="16"/>
+        <v>72</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>87</v>
+      </c>
       <c r="G14" s="16"/>
       <c r="H14" s="16"/>
       <c r="I14" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="30" x14ac:dyDescent="0.2">
       <c r="B15" s="15"/>
       <c r="C15" s="32"/>
       <c r="D15" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="F15" s="16"/>
+        <v>73</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>87</v>
+      </c>
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
       <c r="I15" s="16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J15" s="42" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.2">
@@ -1940,41 +1961,45 @@
     </row>
     <row r="17" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B17" s="39" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="F17" s="16"/>
+        <v>61</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>88</v>
+      </c>
       <c r="G17" s="16"/>
       <c r="H17" s="16"/>
       <c r="I17" s="16" t="s">
         <v>35</v>
       </c>
       <c r="J17" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B18" s="30"/>
       <c r="C18" s="34"/>
       <c r="D18" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37" t="s">
-        <v>80</v>
+        <v>64</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>87</v>
       </c>
       <c r="G18" s="37"/>
       <c r="H18" s="37"/>
       <c r="I18" s="37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J18" s="38"/>
     </row>

</xml_diff>

<commit_message>
add test pport for swc2
</commit_message>
<xml_diff>
--- a/Application.xlsx
+++ b/Application.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutosarTutorial\ArxmlTools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42FEE28B-4174-439C-8E77-C2CEABB8951D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771E2174-7BA9-4BCC-8A01-158D60DE7B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{EBD56D4D-7AAB-47EC-B02E-89E578045FA0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{EBD56D4D-7AAB-47EC-B02E-89E578045FA0}"/>
   </bookViews>
   <sheets>
     <sheet name="DataTypes" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="92">
   <si>
     <t>TypeName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -386,6 +386,14 @@
   </si>
   <si>
     <t>PortName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P_Test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SWC1, Delegation</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1656,10 +1664,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A1755F-5E81-4222-BC5B-9CFC616875A8}">
-  <dimension ref="B1:J19"/>
+  <dimension ref="B1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1870,50 +1878,50 @@
       <c r="I11" s="16"/>
       <c r="J11" s="17"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="4"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="6"/>
-    </row>
-    <row r="13" spans="2:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B13" s="15" t="s">
+    <row r="12" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B12" s="15"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="J12" s="17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B14" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="32" t="s">
+      <c r="C14" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="J13" s="17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B14" s="15"/>
-      <c r="C14" s="32"/>
       <c r="D14" s="16" t="s">
         <v>64</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F14" s="16" t="s">
         <v>87</v>
@@ -1924,17 +1932,17 @@
         <v>74</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" ht="30" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="15" x14ac:dyDescent="0.2">
       <c r="B15" s="15"/>
       <c r="C15" s="32"/>
       <c r="D15" s="16" t="s">
         <v>64</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F15" s="16" t="s">
         <v>87</v>
@@ -1944,75 +1952,96 @@
       <c r="I15" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="J15" s="42" t="s">
+      <c r="J15" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" ht="30" x14ac:dyDescent="0.2">
+      <c r="B16" s="15"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="J16" s="42" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="4"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="6"/>
-    </row>
-    <row r="17" spans="2:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B17" s="39" t="s">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B17" s="4"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="6"/>
+    </row>
+    <row r="18" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B18" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="34" t="s">
+      <c r="C18" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="D18" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E18" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="F17" s="16" t="s">
+      <c r="F18" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16" t="s">
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="J17" s="17" t="s">
+      <c r="J18" s="17" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="2:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="B18" s="30"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="37" t="s">
+    <row r="19" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+      <c r="B19" s="30"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="37" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="37" t="s">
+      <c r="E19" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F19" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37" t="s">
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="J18" s="38"/>
-    </row>
-    <row r="19" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="9"/>
+      <c r="J19" s="38"/>
+    </row>
+    <row r="20" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="7"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>